<commit_message>
Added more hyperparameter configurations
</commit_message>
<xml_diff>
--- a/durations_rg30.xlsx
+++ b/durations_rg30.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>2627.792376041412</v>
+        <v>1586.869649648666</v>
       </c>
     </row>
     <row r="2">
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>304042.6955</v>
+        <v>304042.7785</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>299190</v>
+        <v>306298</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>298905</v>
@@ -465,10 +465,10 @@
         <v>296056</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>102248.8965</v>
+        <v>102244.466</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>100450</v>
+        <v>103074</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>100490</v>

</xml_diff>

<commit_message>
Added futureResourceUtilisation from Xiaolei
</commit_message>
<xml_diff>
--- a/durations_rg30.xlsx
+++ b/durations_rg30.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>1586.869649648666</v>
+        <v>1662.483112335205</v>
       </c>
     </row>
     <row r="2">
@@ -450,7 +450,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>304042.7785</v>
+        <v>304048.0725</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>306298</v>
@@ -465,7 +465,7 @@
         <v>296056</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>102244.466</v>
+        <v>102249.3655</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>103074</v>

</xml_diff>

<commit_message>
Added a combined neural network for main_psplib  -- Not yet working
</commit_message>
<xml_diff>
--- a/durations_rg30.xlsx
+++ b/durations_rg30.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>1662.483112335205</v>
+        <v>2309.938279390335</v>
       </c>
     </row>
     <row r="2">
@@ -450,7 +450,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>304048.0725</v>
+        <v>304048.7895</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>306298</v>
@@ -465,7 +465,7 @@
         <v>296056</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>102249.3655</v>
+        <v>102246.7025</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>103074</v>

</xml_diff>

<commit_message>
Validation set states, actions and futureResourceUtilisationMatrices can now also be extracted from env.py and saved in mains
</commit_message>
<xml_diff>
--- a/durations_rg30.xlsx
+++ b/durations_rg30.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>2382.41220664978</v>
+        <v>2829.552004337311</v>
       </c>
     </row>
     <row r="2">
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>304053.2375</v>
+        <v>304044.503</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>306298</v>
+        <v>299190</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>298905</v>
@@ -465,10 +465,10 @@
         <v>296056</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>102251.8</v>
+        <v>102244.3175</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>103074</v>
+        <v>100450</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>100490</v>

</xml_diff>